<commit_message>
Fix authorization for informal employee, create new table in user repository
</commit_message>
<xml_diff>
--- a/TEEmployee/Files/userDB.xlsx
+++ b/TEEmployee/Files/userDB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="445">
   <si>
     <t>員編</t>
   </si>
@@ -248,6 +248,9 @@
     <t>yswang@mail.sinotech.com.tw</t>
   </si>
   <si>
+    <t>地工組二</t>
+  </si>
+  <si>
     <t>4082</t>
   </si>
   <si>
@@ -362,9 +365,6 @@
     <t>apwang@mail.sinotech.com.tw</t>
   </si>
   <si>
-    <t>地工組二</t>
-  </si>
-  <si>
     <t>4371</t>
   </si>
   <si>
@@ -1347,12 +1347,6 @@
   </si>
   <si>
     <t>weiwen@mail.sinotech.com.tw</t>
-  </si>
-  <si>
-    <t>9991</t>
-  </si>
-  <si>
-    <t>郭薩爾</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:T99"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1518,9 +1512,6 @@
       <c r="R2" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T2" s="0" t="b">
         <v>0</v>
       </c>
@@ -1577,9 +1568,6 @@
       <c r="R3" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S3" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T3" s="0" t="b">
         <v>0</v>
       </c>
@@ -1636,9 +1624,6 @@
       <c r="R4" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S4" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T4" s="0" t="b">
         <v>0</v>
       </c>
@@ -1695,9 +1680,6 @@
       <c r="R5" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S5" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T5" s="0" t="b">
         <v>0</v>
       </c>
@@ -1754,9 +1736,6 @@
       <c r="R6" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S6" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T6" s="0" t="b">
         <v>0</v>
       </c>
@@ -1813,9 +1792,6 @@
       <c r="R7" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S7" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T7" s="0" t="b">
         <v>0</v>
       </c>
@@ -1872,9 +1848,6 @@
       <c r="R8" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S8" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T8" s="0" t="b">
         <v>0</v>
       </c>
@@ -1931,9 +1904,6 @@
       <c r="R9" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S9" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T9" s="0" t="b">
         <v>0</v>
       </c>
@@ -1990,9 +1960,6 @@
       <c r="R10" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S10" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T10" s="0" t="b">
         <v>0</v>
       </c>
@@ -2023,13 +1990,13 @@
         <v>0</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="K11" s="0" t="b">
         <v>0</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="M11" s="0" t="b">
         <v>0</v>
@@ -2048,9 +2015,6 @@
       </c>
       <c r="R11" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S11" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T11" s="0" t="b">
         <v>0</v>
@@ -2058,10 +2022,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>22</v>
@@ -2070,13 +2034,13 @@
         <v>49</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I12" s="0" t="b">
         <v>0</v>
@@ -2108,34 +2072,31 @@
       <c r="R12" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S12" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T12" s="0" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I13" s="0" t="b">
         <v>0</v>
@@ -2147,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M13" s="0" t="b">
         <v>0</v>
@@ -2166,9 +2127,6 @@
       </c>
       <c r="R13" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S13" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T13" s="0" t="b">
         <v>0</v>
@@ -2176,10 +2134,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>22</v>
@@ -2188,13 +2146,13 @@
         <v>49</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I14" s="0" t="b">
         <v>1</v>
@@ -2226,19 +2184,16 @@
       <c r="R14" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S14" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T14" s="0" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>22</v>
@@ -2250,10 +2205,10 @@
         <v>29</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I15" s="0" t="b">
         <v>0</v>
@@ -2265,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M15" s="0" t="b">
         <v>0</v>
@@ -2285,34 +2240,31 @@
       <c r="R15" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S15" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T15" s="0" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I16" s="0" t="b">
         <v>0</v>
@@ -2324,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M16" s="0" t="b">
         <v>0</v>
@@ -2343,9 +2295,6 @@
       </c>
       <c r="R16" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S16" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T16" s="0" t="b">
         <v>0</v>
@@ -2353,10 +2302,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>22</v>
@@ -2368,22 +2317,22 @@
         <v>29</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I17" s="0" t="b">
         <v>0</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="K17" s="0" t="b">
         <v>0</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="M17" s="0" t="b">
         <v>0</v>
@@ -2402,9 +2351,6 @@
       </c>
       <c r="R17" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S17" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T17" s="0" t="b">
         <v>0</v>
@@ -2412,10 +2358,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>22</v>
@@ -2427,10 +2373,10 @@
         <v>29</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I18" s="0" t="b">
         <v>0</v>
@@ -2442,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M18" s="0" t="b">
         <v>0</v>
@@ -2461,9 +2407,6 @@
       </c>
       <c r="R18" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S18" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T18" s="0" t="b">
         <v>0</v>
@@ -2471,10 +2414,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>22</v>
@@ -2486,10 +2429,10 @@
         <v>29</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I19" s="0" t="b">
         <v>0</v>
@@ -2501,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="M19" s="0" t="b">
         <v>1</v>
@@ -2520,9 +2463,6 @@
       </c>
       <c r="R19" s="0" t="b">
         <v>1</v>
-      </c>
-      <c r="S19" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T19" s="0" t="b">
         <v>0</v>
@@ -2560,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M20" s="0" t="b">
         <v>0</v>
@@ -2579,9 +2519,6 @@
       </c>
       <c r="R20" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S20" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T20" s="0" t="b">
         <v>0</v>
@@ -2619,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M21" s="0" t="b">
         <v>0</v>
@@ -2638,9 +2575,6 @@
       </c>
       <c r="R21" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S21" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T21" s="0" t="b">
         <v>0</v>
@@ -2698,9 +2632,6 @@
       <c r="R22" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S22" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T22" s="0" t="b">
         <v>0</v>
       </c>
@@ -2757,9 +2688,6 @@
       <c r="R23" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S23" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T23" s="0" t="b">
         <v>0</v>
       </c>
@@ -2816,9 +2744,6 @@
       <c r="R24" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S24" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T24" s="0" t="b">
         <v>0</v>
       </c>
@@ -2875,9 +2800,6 @@
       <c r="R25" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S25" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T25" s="0" t="b">
         <v>0</v>
       </c>
@@ -2914,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M26" s="0" t="b">
         <v>1</v>
@@ -2933,9 +2855,6 @@
       </c>
       <c r="R26" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S26" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T26" s="0" t="b">
         <v>0</v>
@@ -2993,9 +2912,6 @@
       <c r="R27" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S27" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T27" s="0" t="b">
         <v>0</v>
       </c>
@@ -3032,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M28" s="0" t="b">
         <v>1</v>
@@ -3051,9 +2967,6 @@
       </c>
       <c r="R28" s="0" t="b">
         <v>1</v>
-      </c>
-      <c r="S28" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T28" s="0" t="b">
         <v>0</v>
@@ -3091,7 +3004,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="M29" s="0" t="b">
         <v>0</v>
@@ -3110,9 +3023,6 @@
       </c>
       <c r="R29" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S29" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T29" s="0" t="b">
         <v>0</v>
@@ -3170,9 +3080,6 @@
       <c r="R30" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S30" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T30" s="0" t="b">
         <v>0</v>
       </c>
@@ -3229,9 +3136,6 @@
       <c r="R31" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S31" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T31" s="0" t="b">
         <v>0</v>
       </c>
@@ -3288,9 +3192,6 @@
       <c r="R32" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S32" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T32" s="0" t="b">
         <v>0</v>
       </c>
@@ -3347,9 +3248,6 @@
       <c r="R33" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S33" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T33" s="0" t="b">
         <v>0</v>
       </c>
@@ -3406,9 +3304,6 @@
       <c r="R34" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S34" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T34" s="0" t="b">
         <v>0</v>
       </c>
@@ -3465,9 +3360,6 @@
       <c r="R35" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S35" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T35" s="0" t="b">
         <v>1</v>
       </c>
@@ -3524,9 +3416,6 @@
       <c r="R36" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S36" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T36" s="0" t="b">
         <v>0</v>
       </c>
@@ -3545,7 +3434,7 @@
         <v>49</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>195</v>
@@ -3582,9 +3471,6 @@
       </c>
       <c r="R37" s="0" t="b">
         <v>1</v>
-      </c>
-      <c r="S37" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T37" s="0" t="b">
         <v>0</v>
@@ -3642,9 +3528,6 @@
       <c r="R38" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S38" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T38" s="0" t="b">
         <v>0</v>
       </c>
@@ -3701,9 +3584,6 @@
       <c r="R39" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S39" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T39" s="0" t="b">
         <v>0</v>
       </c>
@@ -3760,9 +3640,6 @@
       <c r="R40" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S40" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T40" s="0" t="b">
         <v>0</v>
       </c>
@@ -3819,9 +3696,6 @@
       <c r="R41" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S41" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T41" s="0" t="b">
         <v>1</v>
       </c>
@@ -3878,9 +3752,6 @@
       <c r="R42" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S42" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T42" s="0" t="b">
         <v>0</v>
       </c>
@@ -3917,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M43" s="0" t="b">
         <v>0</v>
@@ -3936,9 +3807,6 @@
       </c>
       <c r="R43" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S43" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T43" s="0" t="b">
         <v>0</v>
@@ -3996,9 +3864,6 @@
       <c r="R44" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S44" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T44" s="0" t="b">
         <v>0</v>
       </c>
@@ -4035,7 +3900,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M45" s="0" t="b">
         <v>0</v>
@@ -4054,9 +3919,6 @@
       </c>
       <c r="R45" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S45" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T45" s="0" t="b">
         <v>0</v>
@@ -4114,9 +3976,6 @@
       <c r="R46" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S46" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T46" s="0" t="b">
         <v>0</v>
       </c>
@@ -4135,7 +3994,7 @@
         <v>146</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>236</v>
@@ -4172,9 +4031,6 @@
       </c>
       <c r="R47" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S47" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T47" s="0" t="b">
         <v>0</v>
@@ -4232,9 +4088,6 @@
       <c r="R48" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S48" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T48" s="0" t="b">
         <v>0</v>
       </c>
@@ -4291,9 +4144,6 @@
       <c r="R49" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S49" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T49" s="0" t="b">
         <v>1</v>
       </c>
@@ -4350,9 +4200,6 @@
       <c r="R50" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S50" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T50" s="0" t="b">
         <v>0</v>
       </c>
@@ -4409,9 +4256,6 @@
       <c r="R51" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S51" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T51" s="0" t="b">
         <v>0</v>
       </c>
@@ -4442,13 +4286,13 @@
         <v>0</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K52" s="0" t="b">
         <v>0</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="M52" s="0" t="b">
         <v>0</v>
@@ -4467,9 +4311,6 @@
       </c>
       <c r="R52" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S52" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T52" s="0" t="b">
         <v>0</v>
@@ -4527,9 +4368,6 @@
       <c r="R53" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S53" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T53" s="0" t="b">
         <v>0</v>
       </c>
@@ -4586,9 +4424,6 @@
       <c r="R54" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S54" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T54" s="0" t="b">
         <v>0</v>
       </c>
@@ -4645,9 +4480,6 @@
       <c r="R55" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S55" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T55" s="0" t="b">
         <v>0</v>
       </c>
@@ -4663,7 +4495,7 @@
         <v>22</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>29</v>
@@ -4684,7 +4516,7 @@
         <v>0</v>
       </c>
       <c r="L56" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M56" s="0" t="b">
         <v>0</v>
@@ -4703,9 +4535,6 @@
       </c>
       <c r="R56" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S56" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T56" s="0" t="b">
         <v>0</v>
@@ -4763,9 +4592,6 @@
       <c r="R57" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="S57" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T57" s="0" t="b">
         <v>0</v>
       </c>
@@ -4802,7 +4628,7 @@
         <v>0</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M58" s="0" t="b">
         <v>0</v>
@@ -4821,9 +4647,6 @@
       </c>
       <c r="R58" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S58" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T58" s="0" t="b">
         <v>1</v>
@@ -4881,9 +4704,6 @@
       <c r="R59" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S59" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T59" s="0" t="b">
         <v>0</v>
       </c>
@@ -4940,9 +4760,6 @@
       <c r="R60" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S60" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T60" s="0" t="b">
         <v>0</v>
       </c>
@@ -4999,9 +4816,6 @@
       <c r="R61" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S61" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T61" s="0" t="b">
         <v>1</v>
       </c>
@@ -5058,9 +4872,6 @@
       <c r="R62" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S62" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T62" s="0" t="b">
         <v>0</v>
       </c>
@@ -5117,9 +4928,6 @@
       <c r="R63" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S63" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T63" s="0" t="b">
         <v>0</v>
       </c>
@@ -5176,9 +4984,6 @@
       <c r="R64" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S64" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T64" s="0" t="b">
         <v>0</v>
       </c>
@@ -5235,9 +5040,6 @@
       <c r="R65" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S65" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T65" s="0" t="b">
         <v>0</v>
       </c>
@@ -5294,9 +5096,6 @@
       <c r="R66" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S66" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T66" s="0" t="b">
         <v>0</v>
       </c>
@@ -5353,9 +5152,6 @@
       <c r="R67" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S67" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T67" s="0" t="b">
         <v>0</v>
       </c>
@@ -5392,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M68" s="0" t="b">
         <v>0</v>
@@ -5411,9 +5207,6 @@
       </c>
       <c r="R68" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S68" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T68" s="0" t="b">
         <v>0</v>
@@ -5471,9 +5264,6 @@
       <c r="R69" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S69" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T69" s="0" t="b">
         <v>0</v>
       </c>
@@ -5510,7 +5300,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="M70" s="0" t="b">
         <v>0</v>
@@ -5529,9 +5319,6 @@
       </c>
       <c r="R70" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S70" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T70" s="0" t="b">
         <v>0</v>
@@ -5569,7 +5356,7 @@
         <v>0</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M71" s="0" t="b">
         <v>0</v>
@@ -5588,9 +5375,6 @@
       </c>
       <c r="R71" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S71" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T71" s="0" t="b">
         <v>0</v>
@@ -5648,9 +5432,6 @@
       <c r="R72" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S72" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T72" s="0" t="b">
         <v>0</v>
       </c>
@@ -5707,9 +5488,6 @@
       <c r="R73" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S73" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T73" s="0" t="b">
         <v>0</v>
       </c>
@@ -5766,9 +5544,6 @@
       <c r="R74" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S74" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T74" s="0" t="b">
         <v>0</v>
       </c>
@@ -5805,7 +5580,7 @@
         <v>0</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M75" s="0" t="b">
         <v>0</v>
@@ -5824,9 +5599,6 @@
       </c>
       <c r="R75" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S75" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T75" s="0" t="b">
         <v>0</v>
@@ -5884,9 +5656,6 @@
       <c r="R76" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S76" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T76" s="0" t="b">
         <v>0</v>
       </c>
@@ -5943,9 +5712,6 @@
       <c r="R77" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S77" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T77" s="0" t="b">
         <v>0</v>
       </c>
@@ -6002,9 +5768,6 @@
       <c r="R78" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S78" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T78" s="0" t="b">
         <v>0</v>
       </c>
@@ -6061,9 +5824,6 @@
       <c r="R79" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S79" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T79" s="0" t="b">
         <v>0</v>
       </c>
@@ -6100,7 +5860,7 @@
         <v>0</v>
       </c>
       <c r="L80" s="0" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="M80" s="0" t="b">
         <v>0</v>
@@ -6119,9 +5879,6 @@
       </c>
       <c r="R80" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S80" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T80" s="0" t="b">
         <v>0</v>
@@ -6159,7 +5916,7 @@
         <v>0</v>
       </c>
       <c r="L81" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M81" s="0" t="b">
         <v>0</v>
@@ -6178,9 +5935,6 @@
       </c>
       <c r="R81" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S81" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T81" s="0" t="b">
         <v>0</v>
@@ -6238,9 +5992,6 @@
       <c r="R82" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S82" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T82" s="0" t="b">
         <v>0</v>
       </c>
@@ -6297,9 +6048,6 @@
       <c r="R83" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S83" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T83" s="0" t="b">
         <v>0</v>
       </c>
@@ -6336,7 +6084,7 @@
         <v>0</v>
       </c>
       <c r="L84" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M84" s="0" t="b">
         <v>0</v>
@@ -6355,9 +6103,6 @@
       </c>
       <c r="R84" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S84" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T84" s="0" t="b">
         <v>0</v>
@@ -6415,9 +6160,6 @@
       <c r="R85" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S85" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T85" s="0" t="b">
         <v>0</v>
       </c>
@@ -6474,9 +6216,6 @@
       <c r="R86" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S86" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T86" s="0" t="b">
         <v>0</v>
       </c>
@@ -6533,9 +6272,6 @@
       <c r="R87" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S87" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T87" s="0" t="b">
         <v>0</v>
       </c>
@@ -6592,9 +6328,6 @@
       <c r="R88" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S88" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T88" s="0" t="b">
         <v>0</v>
       </c>
@@ -6651,9 +6384,6 @@
       <c r="R89" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S89" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T89" s="0" t="b">
         <v>0</v>
       </c>
@@ -6710,9 +6440,6 @@
       <c r="R90" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S90" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T90" s="0" t="b">
         <v>0</v>
       </c>
@@ -6749,7 +6476,7 @@
         <v>0</v>
       </c>
       <c r="L91" s="0" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="M91" s="0" t="b">
         <v>0</v>
@@ -6768,9 +6495,6 @@
       </c>
       <c r="R91" s="0" t="b">
         <v>0</v>
-      </c>
-      <c r="S91" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="T91" s="0" t="b">
         <v>0</v>
@@ -6828,9 +6552,6 @@
       <c r="R92" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S92" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T92" s="0" t="b">
         <v>0</v>
       </c>
@@ -6887,9 +6608,6 @@
       <c r="R93" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S93" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T93" s="0" t="b">
         <v>0</v>
       </c>
@@ -6946,9 +6664,6 @@
       <c r="R94" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="S94" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="T94" s="0" t="b">
         <v>0</v>
       </c>
@@ -6978,14 +6693,26 @@
       <c r="I95" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="J95" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="K95" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="L95" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="M95" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="N95" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="O95" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="P95" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="Q95" s="0" t="b">
         <v>0</v>
@@ -7022,14 +6749,26 @@
       <c r="I96" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="J96" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="K96" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="L96" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="M96" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="N96" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="O96" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="P96" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="Q96" s="0" t="b">
         <v>0</v>
@@ -7066,14 +6805,26 @@
       <c r="I97" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="J97" s="0" t="s">
+        <v>58</v>
+      </c>
       <c r="K97" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="L97" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="M97" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="N97" s="0" t="s">
+        <v>214</v>
+      </c>
       <c r="O97" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="P97" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="Q97" s="0" t="b">
         <v>0</v>
@@ -7110,15 +6861,27 @@
       <c r="I98" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="J98" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="K98" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="L98" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="M98" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="N98" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="O98" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="P98" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="Q98" s="0" t="b">
         <v>0</v>
       </c>
@@ -7126,56 +6889,6 @@
         <v>0</v>
       </c>
       <c r="T98" s="0" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>446</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="I99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J99" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="K99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="L99" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="M99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="O99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="P99" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="R99" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="S99" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="T99" s="0" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>